<commit_message>
changed the image output
</commit_message>
<xml_diff>
--- a/demo_test_results.xlsx
+++ b/demo_test_results.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
-    <t>Quadratics</t>
+    <t>Unit Test</t>
   </si>
   <si>
     <t>Student</t>
@@ -30,40 +30,40 @@
     <t>Equations</t>
   </si>
   <si>
-    <t>Complete square to solve (MGSE9-12.A.REI.4a )</t>
-  </si>
-  <si>
-    <t>Solve Quadratic Equations by Various Methods (MGSE9-12.A.REI.4b )</t>
-  </si>
-  <si>
-    <t>Graph Equations (MGSE9-12.A.CED.2)</t>
+    <t>Topic 1 (MGSE9-12.A.REI.4a )</t>
+  </si>
+  <si>
+    <t>Topic 2 (MGSE9-12.A.REI.4b )</t>
+  </si>
+  <si>
+    <t>Topic 3 (MGSE9-12.A.CED.2)</t>
   </si>
   <si>
     <t>Expressions</t>
   </si>
   <si>
-    <t>Terms and Factors (MGSE9-12.A.SSE.1a )</t>
-  </si>
-  <si>
-    <t>Factor quadratic expression (MGSE9-12.A.SSE.3a )</t>
+    <t>Topic 4 (MGSE9-12.A.SSE.1a )</t>
+  </si>
+  <si>
+    <t>Topic 5 (MGSE9-12.A.SSE.3a )</t>
   </si>
   <si>
     <t>Functions</t>
   </si>
   <si>
-    <t>Appropriate domain (MGSE9-12.F.IF.5 )</t>
-  </si>
-  <si>
-    <t>Average rate of change (MGSE9-12.F.IF.6 )</t>
-  </si>
-  <si>
-    <t>Graph Functions (MGSE9-12.F.IF.7 )</t>
-  </si>
-  <si>
-    <t>Show zeros, extrema, symmetry (MGSE9-12.F.IF.8a )</t>
-  </si>
-  <si>
-    <t>Transform graphs (MGSE9-12.F.BF.3 )</t>
+    <t>Topic 6 (MGSE9-12.F.IF.5 )</t>
+  </si>
+  <si>
+    <t>Topic 7 (MGSE9-12.F.IF.6 )</t>
+  </si>
+  <si>
+    <t>Topic 8 (MGSE9-12.F.IF.7 )</t>
+  </si>
+  <si>
+    <t>Topic 9 (MGSE9-12.F.IF.8a )</t>
+  </si>
+  <si>
+    <t>Topic 10 (MGSE9-12.F.BF.3 )</t>
   </si>
   <si>
     <t>Student Average</t>
@@ -450,40 +450,40 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>